<commit_message>
Added team member names and emails and resubmitted
</commit_message>
<xml_diff>
--- a/ProgressTrackingSheet.xlsx
+++ b/ProgressTrackingSheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t xml:space="preserve">Team:</t>
   </si>
@@ -32,6 +32,18 @@
   </si>
   <si>
     <t xml:space="preserve">2 hrs/day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team members:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hannes Þór Sveinbjörnsson (hths17@hi.is)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ragnheiður Ásta Karlsdóttir (rak4@hi.is)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viktor Alex Brynjarsson (vab18@hi.is)</t>
   </si>
   <si>
     <t xml:space="preserve">Sprint</t>
@@ -273,25 +285,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M15" activeCellId="0" sqref="M15"/>
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.2397959183674"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.7551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.0459183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="61.5561224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.7551020408163"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="0"/>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
@@ -301,109 +316,79 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0"/>
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="C2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="7" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0"/>
+      <c r="C3" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="6" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0"/>
+      <c r="C4" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="6" t="s">
+    </row>
+    <row r="6" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="B6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="D6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="n">
+      <c r="E6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E6" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B7" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>14</v>
-      </c>
       <c r="D7" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="C8" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="C8" s="8" t="s">
+        <v>16</v>
+      </c>
       <c r="D8" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E8" s="1" t="n">
         <v>10</v>
@@ -414,81 +399,81 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E9" s="1" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>18</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="C12" s="0" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B11" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" s="1" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B12" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>19</v>
-      </c>
       <c r="D12" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E12" s="1" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" s="1" t="n">
         <v>20</v>
@@ -496,16 +481,16 @@
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>20</v>
@@ -513,36 +498,36 @@
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B15" s="1" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" s="1" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16" s="1" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -550,16 +535,16 @@
         <v>2</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="E17" s="1" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -567,30 +552,30 @@
         <v>2</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D18" s="1" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E18" s="1" t="n">
         <v>30</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E19" s="1" t="n">
         <v>30</v>
@@ -601,83 +586,92 @@
         <v>2</v>
       </c>
       <c r="B20" s="1" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>8</v>
+        <v>0.5</v>
       </c>
       <c r="E20" s="1" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="B21" s="1" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D21" s="1" t="n">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="E21" s="1" t="n">
         <v>30</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="B22" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E22" s="1" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="E23" s="1" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E24" s="1" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E22" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D23" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E23" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E24" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>32</v>
+      <c r="C25" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="E25" s="1" t="n">
         <v>40</v>
@@ -685,43 +679,85 @@
     </row>
     <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E26" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E27" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="E28" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="1" t="n">
+      <c r="C29" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="E26" s="1" t="n">
+      <c r="E29" s="1" t="n">
         <v>50</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="1" t="n">
+    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" s="1" t="n">
+      <c r="C30" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="E27" s="1" t="n">
+      <c r="E30" s="1" t="n">
         <v>50</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="1" t="n">
+    <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D28" s="1" t="n">
+      <c r="C31" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E28" s="1" t="n">
+      <c r="E31" s="1" t="n">
         <v>50</v>
       </c>
     </row>

</xml_diff>